<commit_message>
Agregando actividad 2 de Modulo 1_ CANVAS
</commit_message>
<xml_diff>
--- a/Methodology Canvas_Ibarra_Sergio.xlsx
+++ b/Methodology Canvas_Ibarra_Sergio.xlsx
@@ -8,29 +8,39 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\llell\Documents\SIR_Personal\Diplomado_DC_UNAM\Diplomado_DC_UNAM_Full\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{928F07AD-1796-4DEC-A325-BB8C485ACC80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C6A9E7B-7960-4CE1-A3CE-1086940CDFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Problem Statement" sheetId="1" r:id="rId1"/>
     <sheet name="Business Model" sheetId="2" r:id="rId2"/>
     <sheet name="ML Canvas" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="85">
   <si>
     <t>THE PROBLEM STATEMENT CANVAS</t>
   </si>
   <si>
     <t>STARTUP NAME</t>
-  </si>
-  <si>
-    <t>[Type here]</t>
   </si>
   <si>
     <t>DATE</t>
@@ -246,6 +256,55 @@
   </si>
   <si>
     <t>GAS NATURAL S.A de C.V</t>
+  </si>
+  <si>
+    <t>La Secretaria de Energía tiene compendios anuales de Forecast de Gas Natural y del comportamiento del sistema en general, que me permiten estudiarlo en su estado actual</t>
+  </si>
+  <si>
+    <t>Como todo modelo de Forecast la mejor manera de evaluarlo será evaluado el error en el pronóstico, ya sea de tipo MAE, MAPE, etc</t>
+  </si>
+  <si>
+    <t>El modelo creado de Neural Networks (NN) y Time Series puede ser alimentado mensualmente conforme se tengan datos reales, para que dihco modelo, pronostique los siguientes 12-24 meses</t>
+  </si>
+  <si>
+    <t>Doctor_en_casa</t>
+  </si>
+  <si>
+    <t>Servicio de atención medica basica y especializada a domicilio a demanda.
+La idea es que todos podemos necesitar de un buen medico y/o especialista y a veces es complicado tener uno de confianza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ofrecer una plataforma confiable para contactar y agendar citas medicas a domicilio </t>
+  </si>
+  <si>
+    <t>Recursos humanos:
+-Medicos y/o especialistas dispuestos a trabajar en alianza con la plataforma
+-Personal administratrivo y de ventas
+-Personal de programación y sistemas</t>
+  </si>
+  <si>
+    <t>-Empresas que puedan ofrecer a sus trabajadores el beneficio con un descuento
+-Medicos y/o asociaciones de profesionales de la salud
+-Empresas farmaceuticas</t>
+  </si>
+  <si>
+    <t>Lo más relevante para el negocio es la confianza que pueda generar la plataforma</t>
+  </si>
+  <si>
+    <t>Inseguros y desconfiados sobre obtener un excelente servicio a un precio justo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-Empresas 
+-Personas individuales
+</t>
+  </si>
+  <si>
+    <t>La empresa cobraría un aproximado de 15-20% de comisión por consulta acordada y tendra gastos de administración, tecnología y costumer service, entre otros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-De la comisión por consulta
+-De partnership con empresas 
+-De partnership con farmceuticas </t>
   </si>
 </sst>
 </file>
@@ -561,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -626,10 +685,17 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -640,43 +706,8 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -697,26 +728,60 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1038,8 +1103,8 @@
   </sheetPr>
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
@@ -1054,36 +1119,36 @@
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" ht="12.75">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="12.75">
+      <c r="A3" s="26"/>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="12.75">
-      <c r="A3" s="55"/>
-      <c r="B3" s="2" t="s">
+    <row r="4" spans="1:3" ht="12.75">
+      <c r="A4" s="26"/>
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="12.75">
-      <c r="A4" s="55"/>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="54">
+      <c r="C4" s="23">
         <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="24.6" customHeight="1">
-      <c r="A5" s="55"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
@@ -1094,90 +1159,90 @@
     </row>
     <row r="7" spans="1:3" ht="12.75">
       <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>6</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="12.75">
       <c r="A8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="22" t="s">
         <v>9</v>
-      </c>
-      <c r="C8" s="53" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="299.25" customHeight="1">
       <c r="A9" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>56</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="12.75">
       <c r="A10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="12.75">
       <c r="A11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="C11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="14" t="s">
+    </row>
+    <row r="12" spans="1:3" ht="141.75">
+      <c r="A12" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="12.75">
+      <c r="A13" s="28"/>
+      <c r="B13" s="15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="141.75">
-      <c r="A12" s="24" t="s">
+      <c r="C13" s="31"/>
+    </row>
+    <row r="14" spans="1:3" ht="12.75">
+      <c r="A14" s="28"/>
+      <c r="B14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="31"/>
+    </row>
+    <row r="15" spans="1:3" ht="141.75" customHeight="1">
+      <c r="A15" s="29"/>
+      <c r="B15" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="12.75">
-      <c r="A13" s="25"/>
-      <c r="B13" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="28"/>
-    </row>
-    <row r="14" spans="1:3" ht="12.75">
-      <c r="A14" s="25"/>
-      <c r="B14" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="28"/>
-    </row>
-    <row r="15" spans="1:3" ht="141.75" customHeight="1">
-      <c r="A15" s="26"/>
-      <c r="B15" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="29"/>
+      <c r="C15" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1196,8 +1261,8 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
@@ -1217,39 +1282,39 @@
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:6" ht="12.75">
-      <c r="A2" s="22" t="s">
-        <v>19</v>
+      <c r="A2" s="25" t="s">
+        <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="12.75">
+      <c r="A3" s="33"/>
+      <c r="D3" s="2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="12.75">
-      <c r="A3" s="23"/>
-      <c r="D3" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="3" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75">
-      <c r="A4" s="23"/>
+      <c r="A4" s="33"/>
       <c r="D4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="3" t="s">
-        <v>2</v>
+      <c r="F4" s="23">
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="58.9" customHeight="1">
-      <c r="A5" s="23"/>
+      <c r="A5" s="33"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1262,186 +1327,180 @@
     </row>
     <row r="7" spans="1:6" ht="18" customHeight="1" thickTop="1">
       <c r="A7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="D7" s="36"/>
+      <c r="E7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="44"/>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="25.9" customHeight="1">
       <c r="A8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="38"/>
+      <c r="E8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="94.5" customHeight="1" thickBot="1">
+      <c r="A9" s="57" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="40"/>
+      <c r="E9" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="57" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="13.9" customHeight="1" thickTop="1">
+      <c r="A10" s="34"/>
+      <c r="B10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="39"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="34"/>
+    </row>
+    <row r="11" spans="1:6" ht="12.75">
+      <c r="A11" s="34"/>
+      <c r="B11" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="46"/>
-      <c r="E8" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="17" t="s">
+      <c r="C11" s="39"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="34"/>
+    </row>
+    <row r="12" spans="1:6" ht="21" customHeight="1">
+      <c r="A12" s="34"/>
+      <c r="B12" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="39"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" s="34"/>
+    </row>
+    <row r="13" spans="1:6" ht="13.15" customHeight="1">
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+    </row>
+    <row r="14" spans="1:6" ht="13.15" customHeight="1">
+      <c r="A14" s="34"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+    </row>
+    <row r="15" spans="1:6" ht="48.75" customHeight="1" thickBot="1">
+      <c r="A15" s="34"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A16" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="42"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="42"/>
+      <c r="F16" s="43"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A17" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="45"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="44" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="94.5" customHeight="1" thickBot="1">
-      <c r="A9" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="47" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="30" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="13.9" customHeight="1" thickTop="1">
-      <c r="A10" s="30"/>
-      <c r="B10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="30"/>
-    </row>
-    <row r="11" spans="1:6" ht="12.75">
-      <c r="A11" s="30"/>
-      <c r="B11" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="30"/>
-    </row>
-    <row r="12" spans="1:6" ht="21" customHeight="1">
-      <c r="A12" s="30"/>
-      <c r="B12" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="47"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="30"/>
-    </row>
-    <row r="13" spans="1:6" ht="13.15" customHeight="1">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-    </row>
-    <row r="14" spans="1:6" ht="13.15" customHeight="1">
-      <c r="A14" s="30"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-    </row>
-    <row r="15" spans="1:6" ht="48.75" customHeight="1" thickBot="1">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A16" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="32"/>
-      <c r="F16" s="33"/>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A17" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="35"/>
-      <c r="F17" s="36"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="46"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A18" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="38"/>
-      <c r="F18" s="39"/>
+      <c r="A18" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="48"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="58" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="48"/>
+      <c r="F18" s="49"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A19" s="37"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="39"/>
+      <c r="A19" s="47"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="49"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A20" s="37"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="39"/>
+      <c r="A20" s="47"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="49"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A21" s="40"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="42"/>
+      <c r="A21" s="50"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A9:A15"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D15"/>
-    <mergeCell ref="B12:B15"/>
     <mergeCell ref="E12:E15"/>
     <mergeCell ref="F9:F15"/>
     <mergeCell ref="A16:C16"/>
@@ -1450,6 +1509,12 @@
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="D18:F21"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A9:A15"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D15"/>
+    <mergeCell ref="B12:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1462,8 +1527,8 @@
   </sheetPr>
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="134" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
@@ -1483,43 +1548,43 @@
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:6" ht="12.75">
-      <c r="A2" s="22" t="s">
-        <v>36</v>
+      <c r="A2" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75">
-      <c r="A3" s="23"/>
+      <c r="A3" s="33"/>
       <c r="D3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="3" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75">
-      <c r="A4" s="23"/>
+      <c r="A4" s="33"/>
       <c r="D4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="3" t="s">
-        <v>2</v>
+      <c r="F4" s="23">
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="58.9" customHeight="1">
-      <c r="A5" s="23"/>
+      <c r="A5" s="33"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="56"/>
+      <c r="E5" s="24"/>
     </row>
     <row r="6" spans="1:6" ht="34.5" thickBot="1">
       <c r="A6" s="1"/>
@@ -1529,181 +1594,181 @@
     </row>
     <row r="7" spans="1:6" ht="18" customHeight="1" thickTop="1">
       <c r="A7" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="44"/>
+        <v>38</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="36"/>
       <c r="E7" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="47.45" customHeight="1">
       <c r="A8" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="D8" s="54"/>
+      <c r="E8" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="52"/>
-      <c r="E8" s="20" t="s">
+      <c r="F8" s="20" t="s">
         <v>49</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="94.5" customHeight="1" thickBot="1">
       <c r="A9" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="40"/>
+      <c r="E9" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="12" t="s">
+      <c r="F9" s="11" t="s">
         <v>66</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.9" customHeight="1" thickTop="1">
       <c r="A10" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="48"/>
+        <v>39</v>
+      </c>
+      <c r="C10" s="39"/>
+      <c r="D10" s="40"/>
       <c r="E10" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="55.9" customHeight="1">
       <c r="A11" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="C11" s="39"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="19" t="s">
+      <c r="F11" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="21" t="s">
+    </row>
+    <row r="12" spans="1:6" ht="21" customHeight="1">
+      <c r="A12" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="39"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="55" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="13.15" customHeight="1">
+      <c r="A13" s="55"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="55"/>
+    </row>
+    <row r="14" spans="1:6" ht="13.15" customHeight="1">
+      <c r="A14" s="55"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="55"/>
+    </row>
+    <row r="15" spans="1:6" ht="48.75" customHeight="1" thickBot="1">
+      <c r="A15" s="55"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="55"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A16" s="55"/>
+      <c r="B16" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="55"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A17" s="55"/>
+      <c r="B17" s="44" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="21" customHeight="1">
-      <c r="A12" s="49" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="47"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="47" t="s">
-        <v>68</v>
-      </c>
-      <c r="F12" s="49" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="13.15" customHeight="1">
-      <c r="A13" s="49"/>
-      <c r="B13" s="48"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="49"/>
-    </row>
-    <row r="14" spans="1:6" ht="13.15" customHeight="1">
-      <c r="A14" s="49"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="49"/>
-    </row>
-    <row r="15" spans="1:6" ht="48.75" customHeight="1" thickBot="1">
-      <c r="A15" s="49"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="49"/>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A16" s="49"/>
-      <c r="B16" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="49"/>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A17" s="49"/>
-      <c r="B17" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="49"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="55"/>
     </row>
     <row r="18" spans="1:6" ht="58.9" customHeight="1">
-      <c r="A18" s="49"/>
-      <c r="B18" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="49"/>
+      <c r="A18" s="55"/>
+      <c r="B18" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="55"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A19" s="50"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="50"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D15"/>
-    <mergeCell ref="B12:B15"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B18:E19"/>
     <mergeCell ref="A12:A19"/>
     <mergeCell ref="F12:F19"/>
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="E12:E15"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D15"/>
+    <mergeCell ref="B12:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>